<commit_message>
Act jornada 9 partidos aplazados y qr enlace web
</commit_message>
<xml_diff>
--- a/data/clasf_jor10_gA.xlsx
+++ b/data/clasf_jor10_gA.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9282A88-17C5-4B84-9F67-815F88181C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{577E7528-AE9C-4F59-B114-AD12DB3FD5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>PJ</t>
   </si>
   <si>
+    <t>Kero</t>
+  </si>
+  <si>
     <t>Lope</t>
-  </si>
-  <si>
-    <t>Kero</t>
   </si>
   <si>
     <t>Palop</t>
@@ -438,7 +438,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -500,19 +500,19 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -613,10 +613,10 @@
         <v>27</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -626,6 +626,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H7">
+    <sortCondition descending="1" ref="B2:B7"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>